<commit_message>
Update 1 radiance input
</commit_message>
<xml_diff>
--- a/Data Analysis/Results Maehongsorn.xlsx
+++ b/Data Analysis/Results Maehongsorn.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13275" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All input" sheetId="1" r:id="rId1"/>
+    <sheet name="1 input" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Model</t>
   </si>
@@ -263,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -284,9 +285,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -625,115 +623,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.75" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.25" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.25" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.25" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="12" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="18" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="19"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>20</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>2</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>32</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>0.8</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>4</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>32</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <v>18</v>
       </c>
       <c r="J3" s="5">
@@ -742,33 +740,35 @@
       <c r="K3" s="6">
         <v>0.1</v>
       </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="27" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>20</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>32</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>0.8</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>4</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>32</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>18</v>
       </c>
       <c r="J4" s="5">
@@ -777,33 +777,35 @@
       <c r="K4" s="6">
         <v>0.11</v>
       </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="27" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>20</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>128</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>0.8</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>4</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>32</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>18</v>
       </c>
       <c r="J5" s="5">
@@ -812,93 +814,176 @@
       <c r="K5" s="6">
         <v>9.0338000000000002E-2</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <v>5.6972000000000002E-2</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="13">
         <v>4.0400999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:13" ht="27" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>20</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>2</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>128</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>0.8</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>4</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>32</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>18</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="5">
         <v>7.8656000000000004E-2</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="6">
         <v>8.4941000000000003E-2</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <v>5.5469999999999998E-2</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="13">
         <v>3.9468999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="10">
+    <row r="7" spans="1:13" ht="27" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>20</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>128</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>0.8</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>4</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>32</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>18</v>
       </c>
+      <c r="J7" s="5">
+        <v>7.0327000000000001E-2</v>
+      </c>
+      <c r="K7" s="6">
+        <v>6.9386000000000003E-2</v>
+      </c>
+      <c r="L7" s="13">
+        <v>5.5052999999999998E-2</v>
+      </c>
+      <c r="M7" s="13">
+        <v>4.0516999999999997E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+    <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C8" s="9">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10">
+        <v>128</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="9">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9">
+        <v>32</v>
+      </c>
+      <c r="I8" s="9">
+        <v>18</v>
+      </c>
+      <c r="J8" s="5">
+        <v>6.9890999999999995E-2</v>
+      </c>
+      <c r="K8" s="6">
+        <v>6.6647999999999999E-2</v>
+      </c>
+      <c r="L8" s="13">
+        <v>5.5178999999999999E-2</v>
+      </c>
+      <c r="M8" s="13">
+        <v>3.9709000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10">
+        <v>4</v>
+      </c>
+      <c r="E9" s="10">
+        <v>256</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="9">
+        <v>4</v>
+      </c>
+      <c r="H9" s="9">
+        <v>32</v>
+      </c>
+      <c r="I9" s="9">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2">
+        <v>6.3452999999999996E-2</v>
+      </c>
+      <c r="K9" s="3">
+        <v>6.4911999999999997E-2</v>
+      </c>
+      <c r="L9" s="12">
+        <v>5.3531000000000002E-2</v>
+      </c>
+      <c r="M9" s="12">
+        <v>4.1203999999999998E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -914,7 +999,175 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="C1:C2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="J1:J2 J10:J1048576">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F1C933F6-36E5-491C-B289-51EA0DE667CD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K2 K10:K1048576">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A4754CFB-AFA7-49E1-B81B-26542CE7AD38}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L2 L10:L1048576">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{10BCF4A9-C944-4D1F-8A1F-CBD024A29FDD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M2 M10:M1048576">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7B8A57A4-1D8A-4260-8076-DB0E760D11C5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J7 J9">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0C051FFE-C2B0-403E-AD4C-673FFF098F67}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K7 K9">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5DDB3C80-9D6E-4239-B2EA-01C1B4743EB5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L7 L9">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6DB1EB64-59D7-4248-AA1E-0E063CF5FF84}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M7 M9">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6463843D-CC37-49D5-906C-3F4995E31764}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8337BC82-130F-4BF1-8FB5-D79A47E834DC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B548DC97-8A19-46C0-BA1E-B4337789F583}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EF5F24D1-4D23-4176-8BD6-AEFA8B9698EF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AD8C4A34-159F-4C7D-AF18-0044A3CDA152}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J9">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -923,40 +1176,40 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F1C933F6-36E5-491C-B289-51EA0DE667CD}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
+          <x14:id>{07F2CFB5-DF84-494F-87B9-BF88EB150648}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L9">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F2D2C2A8-4874-43A7-9577-D3F6B817522A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K9">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFFF555A"/>
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A4754CFB-AFA7-49E1-B81B-26542CE7AD38}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{10BCF4A9-C944-4D1F-8A1F-CBD024A29FDD}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048576">
+          <x14:id>{9AB9F4C1-A118-49A1-A66C-1246D2E9EAB1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M9">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -965,7 +1218,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7B8A57A4-1D8A-4260-8076-DB0E760D11C5}</x14:id>
+          <x14:id>{4414D5D0-99D9-496A-9B56-ABB166DB5371}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -986,7 +1239,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>J1:J2 J10:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4754CFB-AFA7-49E1-B81B-26542CE7AD38}">
@@ -999,7 +1252,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K1:K1048576</xm:sqref>
+          <xm:sqref>K1:K2 K10:K1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{10BCF4A9-C944-4D1F-8A1F-CBD024A29FDD}">
@@ -1012,7 +1265,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L1:L1048576</xm:sqref>
+          <xm:sqref>L1:L2 L10:L1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7B8A57A4-1D8A-4260-8076-DB0E760D11C5}">
@@ -1025,10 +1278,178 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M1:M1048576</xm:sqref>
+          <xm:sqref>M1:M2 M10:M1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0C051FFE-C2B0-403E-AD4C-673FFF098F67}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J3:J7 J9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5DDB3C80-9D6E-4239-B2EA-01C1B4743EB5}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3:K7 K9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6DB1EB64-59D7-4248-AA1E-0E063CF5FF84}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L3:L7 L9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6463843D-CC37-49D5-906C-3F4995E31764}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M7 M9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8337BC82-130F-4BF1-8FB5-D79A47E834DC}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B548DC97-8A19-46C0-BA1E-B4337789F583}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EF5F24D1-4D23-4176-8BD6-AEFA8B9698EF}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AD8C4A34-159F-4C7D-AF18-0044A3CDA152}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{07F2CFB5-DF84-494F-87B9-BF88EB150648}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J3:J9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F2D2C2A8-4874-43A7-9577-D3F6B817522A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>L3:L9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9AB9F4C1-A118-49A1-A66C-1246D2E9EAB1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3:K9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4414D5D0-99D9-496A-9B56-ABB166DB5371}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M3:M9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>